<commit_message>
ebay_scraping demo version completed
</commit_message>
<xml_diff>
--- a/Boxing/Boxing_Sold_Data_Final.xlsx
+++ b/Boxing/Boxing_Sold_Data_Final.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -1618,8 +1618,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1695,6 +1695,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1773,6 +1778,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1807,6 +1813,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1982,14 +1989,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G195"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A168" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+    <col min="5" max="5" width="43.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2012,7 +2028,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2029,7 +2045,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2049,7 +2065,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2069,7 +2085,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2089,7 +2105,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -2109,7 +2125,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -2126,7 +2142,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -2143,7 +2159,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2163,7 +2179,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -2183,7 +2199,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -2200,7 +2216,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -2220,7 +2236,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -2243,7 +2259,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -2263,7 +2279,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -2286,7 +2302,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -2306,7 +2322,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -2329,7 +2345,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -2352,7 +2368,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -2372,7 +2388,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -2392,7 +2408,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -2412,7 +2428,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -2432,7 +2448,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -2452,7 +2468,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -2472,7 +2488,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -2486,7 +2502,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -2506,7 +2522,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -2529,7 +2545,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -2552,7 +2568,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -2572,7 +2588,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -2595,7 +2611,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -2615,7 +2631,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>13</v>
       </c>
@@ -2638,7 +2654,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>13</v>
       </c>
@@ -2658,7 +2674,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -2681,7 +2697,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>16</v>
       </c>
@@ -2704,7 +2720,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>16</v>
       </c>
@@ -2727,7 +2743,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -2750,7 +2766,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>8</v>
       </c>
@@ -2770,7 +2786,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>8</v>
       </c>
@@ -2790,7 +2806,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>8</v>
       </c>
@@ -2810,7 +2826,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>8</v>
       </c>
@@ -2833,7 +2849,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>8</v>
       </c>
@@ -2856,7 +2872,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>8</v>
       </c>
@@ -2876,7 +2892,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>10</v>
       </c>
@@ -2896,7 +2912,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>8</v>
       </c>
@@ -2919,7 +2935,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>8</v>
       </c>
@@ -2939,7 +2955,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>8</v>
       </c>
@@ -2959,7 +2975,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>13</v>
       </c>
@@ -2982,7 +2998,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>10</v>
       </c>
@@ -3002,7 +3018,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>8</v>
       </c>
@@ -3022,7 +3038,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>8</v>
       </c>
@@ -3042,7 +3058,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>8</v>
       </c>
@@ -3059,7 +3075,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>8</v>
       </c>
@@ -3082,7 +3098,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>8</v>
       </c>
@@ -3105,7 +3121,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>12</v>
       </c>
@@ -3128,7 +3144,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>8</v>
       </c>
@@ -3151,7 +3167,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>17</v>
       </c>
@@ -3171,7 +3187,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>18</v>
       </c>
@@ -3191,7 +3207,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>14</v>
       </c>
@@ -3214,7 +3230,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>8</v>
       </c>
@@ -3237,7 +3253,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>9</v>
       </c>
@@ -3257,7 +3273,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>11</v>
       </c>
@@ -3277,7 +3293,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>14</v>
       </c>
@@ -3297,7 +3313,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>13</v>
       </c>
@@ -3320,7 +3336,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>8</v>
       </c>
@@ -3340,7 +3356,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>8</v>
       </c>
@@ -3363,7 +3379,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>8</v>
       </c>
@@ -3383,7 +3399,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>8</v>
       </c>
@@ -3403,7 +3419,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>13</v>
       </c>
@@ -3426,7 +3442,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>19</v>
       </c>
@@ -3449,7 +3465,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>13</v>
       </c>
@@ -3469,7 +3485,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>13</v>
       </c>
@@ -3492,7 +3508,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>8</v>
       </c>
@@ -3512,7 +3528,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>13</v>
       </c>
@@ -3532,7 +3548,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>8</v>
       </c>
@@ -3552,7 +3568,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>8</v>
       </c>
@@ -3572,7 +3588,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>8</v>
       </c>
@@ -3592,7 +3608,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>8</v>
       </c>
@@ -3612,7 +3628,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>13</v>
       </c>
@@ -3635,7 +3651,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>8</v>
       </c>
@@ -3652,7 +3668,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>8</v>
       </c>
@@ -3672,7 +3688,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>8</v>
       </c>
@@ -3686,7 +3702,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>8</v>
       </c>
@@ -3706,7 +3722,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>8</v>
       </c>
@@ -3726,7 +3742,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>8</v>
       </c>
@@ -3749,7 +3765,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>8</v>
       </c>
@@ -3769,7 +3785,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>8</v>
       </c>
@@ -3789,7 +3805,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>8</v>
       </c>
@@ -3806,7 +3822,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>8</v>
       </c>
@@ -3826,7 +3842,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="90" spans="1:7">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>13</v>
       </c>
@@ -3846,7 +3862,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>8</v>
       </c>
@@ -3869,7 +3885,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="92" spans="1:7">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>8</v>
       </c>
@@ -3889,7 +3905,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>8</v>
       </c>
@@ -3909,7 +3925,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>13</v>
       </c>
@@ -3932,7 +3948,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>8</v>
       </c>
@@ -3943,7 +3959,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="96" spans="1:7">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>8</v>
       </c>
@@ -3954,7 +3970,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="97" spans="1:7">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>12</v>
       </c>
@@ -3974,7 +3990,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="98" spans="1:7">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>20</v>
       </c>
@@ -3997,7 +4013,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="99" spans="1:7">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>8</v>
       </c>
@@ -4017,7 +4033,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="100" spans="1:7">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>21</v>
       </c>
@@ -4034,7 +4050,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="101" spans="1:7">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>10</v>
       </c>
@@ -4057,7 +4073,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="102" spans="1:7">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>16</v>
       </c>
@@ -4077,7 +4093,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="103" spans="1:7">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>8</v>
       </c>
@@ -4097,7 +4113,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="104" spans="1:7">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>13</v>
       </c>
@@ -4120,7 +4136,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="105" spans="1:7">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>8</v>
       </c>
@@ -4140,7 +4156,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="106" spans="1:7">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>13</v>
       </c>
@@ -4160,7 +4176,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="107" spans="1:7">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>8</v>
       </c>
@@ -4177,7 +4193,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="108" spans="1:7">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>8</v>
       </c>
@@ -4194,7 +4210,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="109" spans="1:7">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>13</v>
       </c>
@@ -4217,7 +4233,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="110" spans="1:7">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>9</v>
       </c>
@@ -4240,7 +4256,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="111" spans="1:7">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>9</v>
       </c>
@@ -4260,7 +4276,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="112" spans="1:7">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>9</v>
       </c>
@@ -4280,7 +4296,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="113" spans="1:7">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>9</v>
       </c>
@@ -4300,7 +4316,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="114" spans="1:7">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>9</v>
       </c>
@@ -4320,7 +4336,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="115" spans="1:7">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>9</v>
       </c>
@@ -4340,7 +4356,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="116" spans="1:7">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>22</v>
       </c>
@@ -4360,7 +4376,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="117" spans="1:7">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>23</v>
       </c>
@@ -4383,7 +4399,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="118" spans="1:7">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>9</v>
       </c>
@@ -4403,7 +4419,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="119" spans="1:7">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>9</v>
       </c>
@@ -4423,7 +4439,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="120" spans="1:7">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>23</v>
       </c>
@@ -4443,7 +4459,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="121" spans="1:7">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>23</v>
       </c>
@@ -4466,7 +4482,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="122" spans="1:7">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>8</v>
       </c>
@@ -4480,7 +4496,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="123" spans="1:7">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>12</v>
       </c>
@@ -4491,7 +4507,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="124" spans="1:7">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>13</v>
       </c>
@@ -4514,7 +4530,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="125" spans="1:7">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>13</v>
       </c>
@@ -4534,7 +4550,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="126" spans="1:7">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>8</v>
       </c>
@@ -4554,7 +4570,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="127" spans="1:7">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>13</v>
       </c>
@@ -4577,7 +4593,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="128" spans="1:7">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>8</v>
       </c>
@@ -4597,7 +4613,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="129" spans="1:7">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>8</v>
       </c>
@@ -4617,7 +4633,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="130" spans="1:7">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>13</v>
       </c>
@@ -4637,7 +4653,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="131" spans="1:7">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>8</v>
       </c>
@@ -4657,7 +4673,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="132" spans="1:7">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>13</v>
       </c>
@@ -4680,7 +4696,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="133" spans="1:7">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>8</v>
       </c>
@@ -4703,7 +4719,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="134" spans="1:7">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>8</v>
       </c>
@@ -4720,7 +4736,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="135" spans="1:7">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>13</v>
       </c>
@@ -4740,7 +4756,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="136" spans="1:7">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>8</v>
       </c>
@@ -4751,7 +4767,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="137" spans="1:7">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>8</v>
       </c>
@@ -4771,7 +4787,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="138" spans="1:7">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>8</v>
       </c>
@@ -4794,7 +4810,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="139" spans="1:7">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>12</v>
       </c>
@@ -4805,7 +4821,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="140" spans="1:7">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>8</v>
       </c>
@@ -4825,7 +4841,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="141" spans="1:7">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>8</v>
       </c>
@@ -4845,7 +4861,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="142" spans="1:7">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>8</v>
       </c>
@@ -4865,7 +4881,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="143" spans="1:7">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>13</v>
       </c>
@@ -4888,7 +4904,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="144" spans="1:7">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>13</v>
       </c>
@@ -4908,7 +4924,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="145" spans="1:7">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>13</v>
       </c>
@@ -4931,7 +4947,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="146" spans="1:7">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>8</v>
       </c>
@@ -4954,7 +4970,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="147" spans="1:7">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>12</v>
       </c>
@@ -4977,7 +4993,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="148" spans="1:7">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>12</v>
       </c>
@@ -4988,7 +5004,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="149" spans="1:7">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>12</v>
       </c>
@@ -4999,7 +5015,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="150" spans="1:7">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>8</v>
       </c>
@@ -5019,7 +5035,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="151" spans="1:7">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>8</v>
       </c>
@@ -5039,7 +5055,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="152" spans="1:7">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>8</v>
       </c>
@@ -5056,7 +5072,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="153" spans="1:7">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>13</v>
       </c>
@@ -5076,7 +5092,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="154" spans="1:7">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>8</v>
       </c>
@@ -5099,7 +5115,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="155" spans="1:7">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>24</v>
       </c>
@@ -5119,7 +5135,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="156" spans="1:7">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>8</v>
       </c>
@@ -5139,7 +5155,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="157" spans="1:7">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>8</v>
       </c>
@@ -5159,7 +5175,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="158" spans="1:7">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>8</v>
       </c>
@@ -5170,7 +5186,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="159" spans="1:7">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>8</v>
       </c>
@@ -5190,7 +5206,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="160" spans="1:7">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>13</v>
       </c>
@@ -5210,7 +5226,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="161" spans="1:7">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>12</v>
       </c>
@@ -5233,7 +5249,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="162" spans="1:7">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>8</v>
       </c>
@@ -5253,7 +5269,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="163" spans="1:7">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>8</v>
       </c>
@@ -5273,7 +5289,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="164" spans="1:7">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>8</v>
       </c>
@@ -5293,7 +5309,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="165" spans="1:7">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>8</v>
       </c>
@@ -5313,7 +5329,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="166" spans="1:7">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>8</v>
       </c>
@@ -5333,7 +5349,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="167" spans="1:7">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>13</v>
       </c>
@@ -5356,7 +5372,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="168" spans="1:7">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>8</v>
       </c>
@@ -5376,7 +5392,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="169" spans="1:7">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>12</v>
       </c>
@@ -5387,7 +5403,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="170" spans="1:7">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>13</v>
       </c>
@@ -5410,7 +5426,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="171" spans="1:7">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>10</v>
       </c>
@@ -5433,7 +5449,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="172" spans="1:7">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>11</v>
       </c>
@@ -5453,7 +5469,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="173" spans="1:7">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>8</v>
       </c>
@@ -5473,7 +5489,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="174" spans="1:7">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>8</v>
       </c>
@@ -5493,7 +5509,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="175" spans="1:7">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>8</v>
       </c>
@@ -5516,7 +5532,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="176" spans="1:7">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>8</v>
       </c>
@@ -5533,7 +5549,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="177" spans="1:7">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>25</v>
       </c>
@@ -5556,7 +5572,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="178" spans="1:7">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>8</v>
       </c>
@@ -5576,7 +5592,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="179" spans="1:7">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>8</v>
       </c>
@@ -5596,7 +5612,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="180" spans="1:7">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>8</v>
       </c>
@@ -5619,7 +5635,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="181" spans="1:7">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>8</v>
       </c>
@@ -5639,7 +5655,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="182" spans="1:7">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>13</v>
       </c>
@@ -5662,7 +5678,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="183" spans="1:7">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>13</v>
       </c>
@@ -5685,7 +5701,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="184" spans="1:7">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>8</v>
       </c>
@@ -5705,7 +5721,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="185" spans="1:7">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>13</v>
       </c>
@@ -5728,7 +5744,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="186" spans="1:7">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>10</v>
       </c>
@@ -5751,7 +5767,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="187" spans="1:7">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>8</v>
       </c>
@@ -5771,7 +5787,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="188" spans="1:7">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>13</v>
       </c>
@@ -5794,7 +5810,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="189" spans="1:7">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>13</v>
       </c>
@@ -5817,7 +5833,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="190" spans="1:7">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>13</v>
       </c>
@@ -5840,7 +5856,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="191" spans="1:7">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>13</v>
       </c>
@@ -5863,7 +5879,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="192" spans="1:7">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>13</v>
       </c>
@@ -5883,7 +5899,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="193" spans="1:7">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>8</v>
       </c>
@@ -5906,7 +5922,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="194" spans="1:7">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>13</v>
       </c>
@@ -5929,7 +5945,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="195" spans="1:7">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>12</v>
       </c>

</xml_diff>